<commit_message>
Updated Notebook2 to save figures with embedded fonts, new sizing for publication
</commit_message>
<xml_diff>
--- a/CSVs/Table2.xlsx
+++ b/CSVs/Table2.xlsx
@@ -459,22 +459,22 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>1147.629638090053</v>
+        <v>1147.629638090057</v>
       </c>
       <c r="D2">
-        <v>1.469102276065696e-251</v>
+        <v>1.469102276063019e-251</v>
       </c>
       <c r="E2">
-        <v>2.096058524004447e-250</v>
+        <v>2.096058524000629e-250</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>0.09508145523419442</v>
+        <v>0.09508145523419431</v>
       </c>
       <c r="H2">
-        <v>0.1111800156746186</v>
+        <v>0.1111800156746185</v>
       </c>
       <c r="I2">
         <v>1e-07</v>
@@ -501,10 +501,10 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.07824108450597678</v>
+        <v>0.07824108450597711</v>
       </c>
       <c r="H3">
-        <v>0.08908978742163501</v>
+        <v>0.08908978742163541</v>
       </c>
       <c r="I3">
         <v>1e-07</v>
@@ -519,13 +519,13 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>230.0366290408092</v>
+        <v>230.0366290408056</v>
       </c>
       <c r="D4">
-        <v>5.852674951754162e-52</v>
+        <v>5.852674951764817e-52</v>
       </c>
       <c r="E4">
-        <v>8.350371121678834e-51</v>
+        <v>8.350371121694036e-51</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -549,7 +549,7 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>2101.182149592303</v>
+        <v>2101.182149592307</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -561,10 +561,10 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>0.1591962109497366</v>
+        <v>0.1591962109497363</v>
       </c>
       <c r="H5">
-        <v>0.2129033110426435</v>
+        <v>0.2129033110426433</v>
       </c>
       <c r="I5">
         <v>1e-07</v>
@@ -581,28 +581,28 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>8.554404019567301</v>
+        <v>8.554404019574577</v>
       </c>
       <c r="D6">
-        <v>0.013881447955503</v>
+        <v>0.01388144795545251</v>
       </c>
       <c r="E6">
-        <v>0.1980551510040343</v>
+        <v>0.1980551510033138</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
-        <v>0.0006722969889811914</v>
+        <v>0.0006722969889813024</v>
       </c>
       <c r="H6">
-        <v>0.0007861258495552205</v>
+        <v>0.0007861258495553503</v>
       </c>
       <c r="I6">
-        <v>151.1134424436906</v>
+        <v>151.1134424431409</v>
       </c>
       <c r="J6">
-        <v>0.00661754496376211</v>
+        <v>0.006617544963786183</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -623,10 +623,10 @@
         <v>2</v>
       </c>
       <c r="G7">
-        <v>0.004881393759392227</v>
+        <v>0.004881393759392449</v>
       </c>
       <c r="H7">
-        <v>0.005558234974520695</v>
+        <v>0.005558234974520949</v>
       </c>
       <c r="I7">
         <v>1e-07</v>
@@ -671,22 +671,22 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>101.6381924498855</v>
+        <v>101.6381924498928</v>
       </c>
       <c r="D9">
-        <v>8.502505747871077e-23</v>
+        <v>8.502505747840135e-23</v>
       </c>
       <c r="E9">
-        <v>1.213104760544597e-21</v>
+        <v>1.213104760540182e-21</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9">
-        <v>0.007014034662908397</v>
+        <v>0.007014034662908508</v>
       </c>
       <c r="H9">
-        <v>0.009380318756283446</v>
+        <v>0.009380318756283593</v>
       </c>
       <c r="I9">
         <v>1e-07</v>
@@ -703,10 +703,10 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>2.033493086990347</v>
+        <v>2.033493086993985</v>
       </c>
       <c r="D10">
-        <v>0.1538666126797445</v>
+        <v>0.1538666126793762</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -715,16 +715,16 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0.0001597658752512388</v>
+        <v>0.0001597658752510167</v>
       </c>
       <c r="H10">
-        <v>0.0001868163720354357</v>
+        <v>0.000186816372035176</v>
       </c>
       <c r="I10">
-        <v>37.74563636381713</v>
+        <v>37.74563636374847</v>
       </c>
       <c r="J10">
-        <v>0.0264931286456889</v>
+        <v>0.02649312864573709</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -733,28 +733,28 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>36.99154828471364</v>
+        <v>36.99154828471728</v>
       </c>
       <c r="D11">
-        <v>1.186424018905185e-09</v>
+        <v>1.186424018902972e-09</v>
       </c>
       <c r="E11">
-        <v>1.692744078083928e-08</v>
+        <v>1.69274407808077e-08</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>0.002989366833111351</v>
+        <v>0.002989366833111573</v>
       </c>
       <c r="H11">
-        <v>0.003403864572797843</v>
+        <v>0.003403864572798096</v>
       </c>
       <c r="I11">
-        <v>9.678800013908924e-07</v>
+        <v>9.678800013891319e-07</v>
       </c>
       <c r="J11">
-        <v>1033185.930655608</v>
+        <v>1033185.930657487</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -793,22 +793,22 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>51.38242778730637</v>
+        <v>51.38242778731001</v>
       </c>
       <c r="D13">
-        <v>7.601592128722202e-13</v>
+        <v>7.601592128708124e-13</v>
       </c>
       <c r="E13">
-        <v>1.084565876521777e-11</v>
+        <v>1.084565876519768e-11</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <v>0.003537707726233408</v>
+        <v>0.003537707726233297</v>
       </c>
       <c r="H13">
-        <v>0.004731203612968157</v>
+        <v>0.004731203612968008</v>
       </c>
       <c r="I13">
         <v>1e-07</v>
@@ -825,10 +825,10 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>1.545690702172578</v>
+        <v>1.545690702179854</v>
       </c>
       <c r="D14">
-        <v>0.4616975060801228</v>
+        <v>0.4616975060784431</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -837,16 +837,16 @@
         <v>2</v>
       </c>
       <c r="G14">
-        <v>0.0001214378826756013</v>
+        <v>0.0001214378826753792</v>
       </c>
       <c r="H14">
-        <v>0.000141998938343029</v>
+        <v>0.0001419989383427694</v>
       </c>
       <c r="I14">
-        <v>5026.039051191038</v>
+        <v>5026.039051172754</v>
       </c>
       <c r="J14">
-        <v>0.0001989638341077009</v>
+        <v>0.0001989638341084247</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -867,10 +867,10 @@
         <v>2</v>
       </c>
       <c r="G15">
-        <v>0.0001062402935479989</v>
+        <v>0.000106240293548221</v>
       </c>
       <c r="H15">
-        <v>0.0001209712931200526</v>
+        <v>0.0001209712931203055</v>
       </c>
       <c r="I15">
         <v>5635.414116923059</v>
@@ -885,10 +885,10 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>2.097406492783193</v>
+        <v>2.097406492786831</v>
       </c>
       <c r="D16">
-        <v>0.3503918264996476</v>
+        <v>0.3503918264990103</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -897,16 +897,16 @@
         <v>2</v>
       </c>
       <c r="G16">
-        <v>0.0001823334446464653</v>
+        <v>0.0001823334446470204</v>
       </c>
       <c r="H16">
-        <v>0.000192688642246759</v>
+        <v>0.0001926886422473456</v>
       </c>
       <c r="I16">
-        <v>3814.365423277306</v>
+        <v>3814.365423270368</v>
       </c>
       <c r="J16">
-        <v>0.0002621668060163987</v>
+        <v>0.0002621668060168756</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -915,10 +915,10 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>0.5443031377726584</v>
+        <v>0.5443031377799343</v>
       </c>
       <c r="D17">
-        <v>0.7617387964385844</v>
+        <v>0.7617387964358131</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -933,10 +933,10 @@
         <v>5.000153827441967e-05</v>
       </c>
       <c r="I17">
-        <v>8292.288538035087</v>
+        <v>8292.288538004919</v>
       </c>
       <c r="J17">
-        <v>0.000120593970580401</v>
+        <v>0.0001205939705808398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>